<commit_message>
made an exe version
</commit_message>
<xml_diff>
--- a/Intel_.xlsx
+++ b/Intel_.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>query</t>
   </si>
@@ -146,27 +146,6 @@
   </si>
   <si>
     <t>73.22.194.18</t>
-  </si>
-  <si>
-    <t>6 - geodatatool</t>
-  </si>
-  <si>
-    <t>https://www.geodatatool.com/en/?IP=73.176.21.40</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Success - 200</t>
-  </si>
-  <si>
-    <t>https://www.geodatatool.com/en/?IP=73.22.194.18</t>
-  </si>
-  <si>
-    <t>Oak Lawn</t>
   </si>
 </sst>
 </file>
@@ -529,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN5"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -948,250 +927,6 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
-      <c r="A4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40">
-      <c r="A5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN5" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>